<commit_message>
atualização de muita coisa
</commit_message>
<xml_diff>
--- a/documentos/Tabelas-sistema-bilhetagem.xlsx
+++ b/documentos/Tabelas-sistema-bilhetagem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sis-bilhetagem\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFE33E2-513B-4C73-8F34-AC7E24FC7D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B936F9-E9C8-40DA-B099-C51DB285E2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="24615" windowHeight="11835" tabRatio="760" activeTab="1" xr2:uid="{54C7B9D5-F4B4-46C3-8C81-743BDA97114C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="1" xr2:uid="{54C7B9D5-F4B4-46C3-8C81-743BDA97114C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -101,6 +101,104 @@
         </r>
       </text>
     </comment>
+    <comment ref="G8" authorId="1" shapeId="0" xr:uid="{E717DB50-8468-458A-9157-E4F161C3BEC1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Administrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+datahora q o responsável começou a fazer o pre cadastro. Status=9</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="1" shapeId="0" xr:uid="{402C1AF0-07AB-48C0-A4F3-EED03F630AFE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Administrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+datahora em que o cadastro foi concluido pelo responsávl troca status=9 para status=1
+ou a pre-reserva foi cadastrada no balcao, status=1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="1" shapeId="0" xr:uid="{AE2065B9-0363-450D-BFD2-6EEC9D40C651}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Administrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+horário em que o pagamento é de fato realizado, status=2.
+mesmo horario q começa contar o tempo da entrada</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="1" shapeId="0" xr:uid="{BC203BA7-B2CD-4647-9F0D-6BAA2CA60355}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Administrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+aparentemente criei esse campo a mais sem querer</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E11" authorId="0" shapeId="0" xr:uid="{758475E3-4D54-4914-8185-5EE2DF6498C5}">
       <text>
         <r>
@@ -384,7 +482,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
   <si>
     <t>Perfil</t>
   </si>
@@ -612,6 +710,18 @@
   </si>
   <si>
     <t>autoriza</t>
+  </si>
+  <si>
+    <t>datahora_solicita</t>
+  </si>
+  <si>
+    <t>datahora_efetiva</t>
+  </si>
+  <si>
+    <t>pre_pgtodatahora</t>
+  </si>
+  <si>
+    <t>pre_reservadatahora</t>
   </si>
 </sst>
 </file>
@@ -1102,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A973B4A-3E8B-44A4-899E-BEBEC8825FB8}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,9 +1224,10 @@
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
     <col min="11" max="11" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1190,6 +1301,18 @@
       </c>
       <c r="F8" t="s">
         <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" t="s">
+        <v>79</v>
       </c>
       <c r="M8" t="s">
         <v>27</v>

</xml_diff>